<commit_message>
Get x and y subplot from onRender() in scatMat
</commit_message>
<xml_diff>
--- a/ShinyPlotly/Hex/HexPairs/app-smHex-CurveNumber.xlsx
+++ b/ShinyPlotly/Hex/HexPairs/app-smHex-CurveNumber.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="0" windowWidth="12060" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="17740" yWindow="0" windowWidth="8000" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,11 +205,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -560,8 +567,8 @@
   <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F121" sqref="F121"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -751,13 +758,13 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>16</v>
       </c>
     </row>

</xml_diff>